<commit_message>
Compare ERAInterim - S4 GOTM output for Norway
</commit_message>
<xml_diff>
--- a/Norway_Morsa/Data/Meteorological/04_tercile_plots/seasonal_forecast_performance_1981-2010.xlsx
+++ b/Norway_Morsa/Data/Meteorological/04_tercile_plots/seasonal_forecast_performance_1981-2010.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\niva-of5\osl-userdata$\JES\System\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{216F7690-E067-41CB-8D6A-95C8F5E4B991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4F3427-D7F3-48A9-8B4D-39C76C49B808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{C707A06B-3F10-490C-BDDB-1A1BC2DB9669}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -473,16 +473,16 @@
         <v>10</v>
       </c>
       <c r="C2" s="3">
-        <v>0.25</v>
+        <v>0.47</v>
       </c>
       <c r="D2" s="3">
-        <v>0.16</v>
+        <v>-0.19</v>
       </c>
       <c r="E2" s="3">
-        <v>-0.03</v>
+        <v>0.59</v>
       </c>
       <c r="F2" s="3">
-        <v>-0.16</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -493,16 +493,16 @@
         <v>11</v>
       </c>
       <c r="C3" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.01</v>
       </c>
       <c r="D3" s="3">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E3" s="3">
-        <v>-0.15</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="F3" s="3">
-        <v>-0.32</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -513,13 +513,13 @@
         <v>12</v>
       </c>
       <c r="C4" s="3">
-        <v>0.04</v>
+        <v>0.31</v>
       </c>
       <c r="D4" s="3">
-        <v>0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="E4" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.25</v>
       </c>
       <c r="F4" s="3">
         <v>0.18</v>
@@ -533,16 +533,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>0.32</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D5" s="3">
-        <v>-0.01</v>
+        <v>0.27</v>
       </c>
       <c r="E5" s="3">
-        <v>0.02</v>
+        <v>0.68</v>
       </c>
       <c r="F5" s="3">
-        <v>-0.06</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -553,16 +553,16 @@
         <v>11</v>
       </c>
       <c r="C6" s="3">
-        <v>-7.0000000000000007E-2</v>
+        <v>0.36</v>
       </c>
       <c r="D6" s="3">
-        <v>-0.02</v>
+        <v>-0.15</v>
       </c>
       <c r="E6" s="3">
-        <v>-0.16</v>
+        <v>0.21</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.17</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -573,16 +573,16 @@
         <v>12</v>
       </c>
       <c r="C7" s="3">
-        <v>0.46</v>
+        <v>0.97</v>
       </c>
       <c r="D7" s="3">
-        <v>0.19</v>
+        <v>0.09</v>
       </c>
       <c r="E7" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.72</v>
       </c>
       <c r="F7" s="3">
-        <v>0.01</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -593,16 +593,16 @@
         <v>10</v>
       </c>
       <c r="C8" s="3">
-        <v>0.15</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D8" s="3">
-        <v>0.02</v>
+        <v>0.22</v>
       </c>
       <c r="E8" s="3">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="F8" s="3">
-        <v>-0.06</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -613,16 +613,16 @@
         <v>11</v>
       </c>
       <c r="C9" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D9" s="3">
         <v>0.25</v>
       </c>
-      <c r="D9" s="3">
-        <v>-0.28000000000000003</v>
-      </c>
       <c r="E9" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="F9" s="3">
         <v>-0.05</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -636,13 +636,13 @@
         <v>0.22</v>
       </c>
       <c r="D10" s="3">
-        <v>-0.1</v>
+        <v>0.04</v>
       </c>
       <c r="E10" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.26</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.22</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -653,16 +653,16 @@
         <v>10</v>
       </c>
       <c r="C11" s="3">
-        <v>-0.31</v>
+        <v>0.54</v>
       </c>
       <c r="D11" s="3">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="E11" s="3">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.22</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -673,16 +673,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="3">
-        <v>-0.45</v>
+        <v>-0.72</v>
       </c>
       <c r="D12" s="3">
-        <v>0.34</v>
+        <v>0.23</v>
       </c>
       <c r="E12" s="3">
-        <v>0.18</v>
+        <v>-0.19</v>
       </c>
       <c r="F12" s="3">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -693,16 +693,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="3">
-        <v>-0.22</v>
+        <v>0.13</v>
       </c>
       <c r="D13" s="3">
-        <v>0.48</v>
+        <v>0.68</v>
       </c>
       <c r="E13" s="3">
-        <v>0.05</v>
+        <v>-0.16</v>
       </c>
       <c r="F13" s="3">
-        <v>-0.3</v>
+        <v>-0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>